<commit_message>
updated feature graph code and results
</commit_message>
<xml_diff>
--- a/Features/features_mega_matrix.xlsx
+++ b/Features/features_mega_matrix.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="638" yWindow="480" windowWidth="17978" windowHeight="6878" activeTab="1"/>
+    <workbookView xWindow="638" yWindow="480" windowWidth="17978" windowHeight="6878"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
     <sheet name="Categorical Character Key" sheetId="2" r:id="rId2"/>
     <sheet name="Questionable Columns-- ask Ahme" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1688,7 +1688,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1698,6 +1698,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1742,7 +1748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1776,6 +1782,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2080,67 +2091,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:QI21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="8.796875" style="2"/>
-    <col min="14" max="14" width="18.1328125" customWidth="1"/>
+    <col min="1" max="4" width="8.796875" style="15"/>
+    <col min="5" max="5" width="8.796875" style="2"/>
+    <col min="15" max="15" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:451" s="1" customFormat="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>485</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>509</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>510</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>512</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>513</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>514</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>515</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>516</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>517</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>518</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>487</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>485</v>
       </c>
       <c r="R1" s="9" t="s">
         <v>493</v>
@@ -3446,56 +3458,56 @@
       </c>
     </row>
     <row r="2" spans="1:451" ht="15.75">
-      <c r="A2">
+      <c r="A2" s="15">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C2" s="15">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="15">
+        <v>197</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
-        <v>519</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2" s="3">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="12">
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="12">
         <v>38429</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>38488</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>8.4285714285714288</v>
-      </c>
-      <c r="Q2">
-        <v>197</v>
       </c>
       <c r="R2">
         <v>15420</v>
@@ -4801,56 +4813,56 @@
       </c>
     </row>
     <row r="3" spans="1:451" ht="15.75">
-      <c r="A3">
+      <c r="A3" s="15">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15">
+        <v>5.5714285714285712</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>1555.2</v>
       </c>
-      <c r="J3" t="s">
-        <v>519</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3" s="12">
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="12">
         <v>37620</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>37630</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1.4285714285714286</v>
-      </c>
-      <c r="Q3">
-        <v>5.5714285714285712</v>
       </c>
       <c r="R3">
         <v>1286800</v>
@@ -6156,56 +6168,56 @@
       </c>
     </row>
     <row r="4" spans="1:451" ht="15.75">
-      <c r="A4">
+      <c r="A4" s="15">
         <v>17</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2</v>
+      </c>
+      <c r="D4" s="15">
+        <v>104</v>
+      </c>
+      <c r="E4">
         <v>17</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>60.2</v>
       </c>
-      <c r="J4" t="s">
-        <v>519</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="12">
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="12">
         <v>37995</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>38033</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>5.4285714285714288</v>
-      </c>
-      <c r="Q4">
-        <v>104</v>
       </c>
       <c r="R4">
         <v>39286</v>
@@ -7511,56 +7523,56 @@
       </c>
     </row>
     <row r="5" spans="1:451" ht="15.75">
-      <c r="A5">
+      <c r="A5" s="15">
         <v>20</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C5" s="15">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15">
+        <v>5.5714285714285712</v>
+      </c>
+      <c r="E5">
         <v>20</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
         <v>10.199999999999999</v>
       </c>
-      <c r="J5" t="s">
-        <v>519</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="12">
+      <c r="M5" s="3">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12">
         <v>38015</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>38043</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>4</v>
-      </c>
-      <c r="Q5">
-        <v>5.5714285714285712</v>
       </c>
       <c r="R5">
         <v>24172</v>
@@ -8866,56 +8878,56 @@
       </c>
     </row>
     <row r="6" spans="1:451" ht="15.75">
-      <c r="A6">
+      <c r="A6" s="15">
         <v>48</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15">
+        <v>101.85714285714286</v>
+      </c>
+      <c r="E6">
         <v>48</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>10017.4</v>
       </c>
-      <c r="J6" t="s">
-        <v>519</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6" s="3">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="12">
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
         <v>38754</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>38769</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>2.1428571428571428</v>
-      </c>
-      <c r="Q6">
-        <v>101.85714285714286</v>
       </c>
       <c r="R6">
         <v>1042400</v>
@@ -10221,23 +10233,23 @@
       </c>
     </row>
     <row r="7" spans="1:451" ht="15.75">
-      <c r="A7">
+      <c r="A7" s="15">
         <v>49</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C7" s="15">
+        <v>2</v>
+      </c>
+      <c r="D7" s="15">
+        <v>138.85714285714286</v>
+      </c>
+      <c r="E7">
         <v>49</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -10246,31 +10258,31 @@
         <v>0</v>
       </c>
       <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>1.8</v>
       </c>
-      <c r="J7" t="s">
-        <v>519</v>
-      </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="12">
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" s="12">
         <v>38883</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>38889</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>0.8571428571428571</v>
-      </c>
-      <c r="Q7">
-        <v>138.85714285714286</v>
       </c>
       <c r="R7">
         <v>10746</v>
@@ -11576,56 +11588,56 @@
       </c>
     </row>
     <row r="8" spans="1:451" ht="15.75">
-      <c r="A8">
+      <c r="A8" s="15">
         <v>53</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C8" s="15">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>4.1428571428571432</v>
+      </c>
+      <c r="E8">
         <v>53</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>2</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
         <v>102</v>
       </c>
-      <c r="J8" t="s">
-        <v>519</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8" s="3">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" s="12">
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
         <v>38972</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>38978</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0.8571428571428571</v>
-      </c>
-      <c r="Q8">
-        <v>4.1428571428571432</v>
       </c>
       <c r="R8">
         <v>710310</v>
@@ -12931,23 +12943,23 @@
       </c>
     </row>
     <row r="9" spans="1:451" ht="15.75">
-      <c r="A9">
+      <c r="A9" s="15">
         <v>62</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C9" s="15">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15">
+        <v>229.85714285714286</v>
+      </c>
+      <c r="E9">
         <v>62</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -12956,31 +12968,31 @@
         <v>1</v>
       </c>
       <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J9" t="s">
-        <v>519</v>
-      </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" s="12">
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="12">
         <v>39462</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>39486</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>3.4285714285714284</v>
-      </c>
-      <c r="Q9">
-        <v>229.85714285714286</v>
       </c>
       <c r="R9">
         <v>11663</v>
@@ -14286,56 +14298,56 @@
       </c>
     </row>
     <row r="10" spans="1:451" ht="15.75">
-      <c r="A10">
+      <c r="A10" s="15">
         <v>69</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C10" s="15">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15">
+        <v>96.857142857142861</v>
+      </c>
+      <c r="E10">
         <v>69</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>3</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>6.7</v>
       </c>
-      <c r="J10" t="s">
-        <v>519</v>
-      </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-      <c r="L10" s="3">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="12">
         <v>40347</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>40388</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>5.8571428571428568</v>
-      </c>
-      <c r="Q10">
-        <v>96.857142857142861</v>
       </c>
       <c r="R10">
         <v>21276</v>
@@ -15641,56 +15653,56 @@
       </c>
     </row>
     <row r="11" spans="1:451" ht="15.75">
-      <c r="A11">
+      <c r="A11" s="15">
         <v>70</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <v>6</v>
+      </c>
+      <c r="E11">
         <v>70</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>3</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>6.7</v>
       </c>
-      <c r="J11" t="s">
-        <v>519</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11" s="12">
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11" s="12">
         <v>41248</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>41276</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>4</v>
-      </c>
-      <c r="Q11">
-        <v>6</v>
       </c>
       <c r="R11">
         <v>66280</v>
@@ -16996,56 +17008,56 @@
       </c>
     </row>
     <row r="12" spans="1:451" ht="15.75">
-      <c r="A12">
+      <c r="A12" s="15">
         <v>71</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15">
+        <v>6</v>
+      </c>
+      <c r="E12">
         <v>71</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
         <v>6730.7</v>
       </c>
-      <c r="J12" t="s">
-        <v>519</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" s="3">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" s="12">
+      <c r="M12" s="3">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12">
         <v>39524</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>39534</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>1.4285714285714286</v>
-      </c>
-      <c r="Q12">
-        <v>6</v>
       </c>
       <c r="R12">
         <v>94563</v>
@@ -18351,56 +18363,56 @@
       </c>
     </row>
     <row r="13" spans="1:451" ht="15.75">
-      <c r="A13">
+      <c r="A13" s="15">
         <v>83</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2</v>
+      </c>
+      <c r="D13" s="15">
+        <v>115.71428571428571</v>
+      </c>
+      <c r="E13">
         <v>83</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>3</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>15450.4</v>
       </c>
-      <c r="J13" t="s">
-        <v>519</v>
-      </c>
-      <c r="K13">
-        <v>2</v>
-      </c>
-      <c r="L13" s="4">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" s="12">
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="12">
         <v>39849</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>39864</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>2.1428571428571428</v>
-      </c>
-      <c r="Q13">
-        <v>115.71428571428571</v>
       </c>
       <c r="R13">
         <v>350440</v>
@@ -19706,56 +19718,56 @@
       </c>
     </row>
     <row r="14" spans="1:451" ht="15.75">
-      <c r="A14">
+      <c r="A14" s="15">
         <v>87</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2</v>
+      </c>
+      <c r="D14" s="15">
+        <v>90</v>
+      </c>
+      <c r="E14">
         <v>87</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
         <v>2</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>13.7</v>
       </c>
-      <c r="J14" t="s">
-        <v>519</v>
-      </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
-      <c r="L14" s="3">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" s="12">
+      <c r="M14" s="3">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12">
         <v>39926</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>39952</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>3.7142857142857144</v>
-      </c>
-      <c r="Q14">
-        <v>90</v>
       </c>
       <c r="R14">
         <v>65986</v>
@@ -21061,23 +21073,23 @@
       </c>
     </row>
     <row r="15" spans="1:451" ht="15.75">
-      <c r="A15">
+      <c r="A15" s="15">
         <v>92</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15">
+        <v>9.8571428571428577</v>
+      </c>
+      <c r="E15">
         <v>92</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -21086,31 +21098,31 @@
         <v>1</v>
       </c>
       <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
         <v>38.5</v>
       </c>
-      <c r="J15" t="s">
-        <v>519</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15" s="3">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15" s="12">
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="12">
         <v>40023</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>40043</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>2.8571428571428572</v>
-      </c>
-      <c r="Q15">
-        <v>9.8571428571428577</v>
       </c>
       <c r="R15">
         <v>963530</v>
@@ -22416,56 +22428,56 @@
       </c>
     </row>
     <row r="16" spans="1:451" ht="15.75">
-      <c r="A16">
+      <c r="A16" s="15">
         <v>98</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
+      <c r="D16" s="15">
+        <v>73.571428571428569</v>
+      </c>
+      <c r="E16">
         <v>98</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
         <v>3</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
-        <v>519</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16" s="4">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16" s="12">
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="12">
         <v>40122</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>40151</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>4.1428571428571432</v>
-      </c>
-      <c r="Q16">
-        <v>73.571428571428569</v>
       </c>
       <c r="R16">
         <v>9907</v>
@@ -23771,21 +23783,21 @@
       </c>
     </row>
     <row r="17" spans="1:451" ht="15.75">
-      <c r="A17">
+      <c r="A17" s="15">
         <v>100</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15">
+        <v>4</v>
+      </c>
+      <c r="E17">
         <v>100</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
       <c r="F17">
         <v>0</v>
       </c>
@@ -23796,31 +23808,31 @@
         <v>0</v>
       </c>
       <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>4</v>
       </c>
-      <c r="J17" t="s">
-        <v>519</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17" s="3">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17" s="12">
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17" s="12">
         <v>40163</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>40186</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>3.2857142857142856</v>
-      </c>
-      <c r="Q17">
-        <v>4</v>
       </c>
       <c r="R17">
         <v>294510</v>
@@ -25126,56 +25138,56 @@
       </c>
     </row>
     <row r="18" spans="1:451" ht="15.75">
-      <c r="A18">
+      <c r="A18" s="15">
         <v>102</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C18" s="15">
+        <v>1</v>
+      </c>
+      <c r="D18" s="15">
+        <v>4.8571428571428568</v>
+      </c>
+      <c r="E18">
         <v>102</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
         <v>2</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>7.4</v>
       </c>
-      <c r="J18" t="s">
-        <v>519</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18" s="12">
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18" s="12">
         <v>40183</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>40228</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>6.4285714285714288</v>
-      </c>
-      <c r="Q18">
-        <v>4.8571428571428568</v>
       </c>
       <c r="R18">
         <v>7627</v>
@@ -26481,56 +26493,56 @@
       </c>
     </row>
     <row r="19" spans="1:451" ht="15.75">
-      <c r="A19">
+      <c r="A19" s="15">
         <v>121</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C19" s="15">
+        <v>1</v>
+      </c>
+      <c r="D19" s="15">
+        <v>4.1428571428571432</v>
+      </c>
+      <c r="E19">
         <v>121</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>2278.6</v>
       </c>
-      <c r="J19" t="s">
-        <v>519</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19" s="3">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" s="12">
+      <c r="M19" s="3">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="12">
         <v>40738</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>40764</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>3.7142857142857144</v>
-      </c>
-      <c r="Q19">
-        <v>4.1428571428571432</v>
       </c>
       <c r="R19">
         <v>224040</v>
@@ -27836,56 +27848,56 @@
       </c>
     </row>
     <row r="20" spans="1:451" ht="15.75">
-      <c r="A20">
+      <c r="A20" s="15">
         <v>122</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C20" s="15">
+        <v>1</v>
+      </c>
+      <c r="D20" s="15">
+        <v>6</v>
+      </c>
+      <c r="E20">
         <v>122</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
         <v>58.1</v>
       </c>
-      <c r="J20" t="s">
-        <v>519</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20" s="5">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20" s="12">
+      <c r="M20" s="5">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20" s="12">
         <v>40694</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>40696</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>0.2857142857142857</v>
-      </c>
-      <c r="Q20">
-        <v>6</v>
       </c>
       <c r="R20">
         <v>239470</v>
@@ -29191,56 +29203,56 @@
       </c>
     </row>
     <row r="21" spans="1:451" ht="15.75">
-      <c r="A21">
+      <c r="A21" s="15">
         <v>124</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C21" s="15">
+        <v>2</v>
+      </c>
+      <c r="D21" s="15">
+        <v>80.142857142857139</v>
+      </c>
+      <c r="E21">
         <v>124</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
         <v>2</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
         <v>6.1</v>
       </c>
-      <c r="J21" t="s">
-        <v>519</v>
-      </c>
-      <c r="K21">
-        <v>2</v>
-      </c>
-      <c r="L21" s="3">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21" s="12">
+      <c r="M21" s="3">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="12">
         <v>40812</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>40820</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>1.1428571428571428</v>
-      </c>
-      <c r="Q21">
-        <v>80.142857142857139</v>
       </c>
       <c r="R21">
         <v>126010</v>
@@ -30555,7 +30567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="A75" sqref="A75:A77"/>
     </sheetView>
   </sheetViews>

</xml_diff>